<commit_message>
update customer export and import small bug
</commit_message>
<xml_diff>
--- a/src/main/resources/static/assets/customers.xlsx
+++ b/src/main/resources/static/assets/customers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>姓名</t>
   </si>
@@ -49,7 +49,7 @@
     <t>客户分类</t>
   </si>
   <si>
-    <t>客户备注</t>
+    <t>客户级别</t>
   </si>
   <si>
     <t>张三</t>
@@ -73,12 +73,12 @@
     <t>新建</t>
   </si>
   <si>
+    <t>意向客户</t>
+  </si>
+  <si>
     <t>普通客户</t>
   </si>
   <si>
-    <t>i like it</t>
-  </si>
-  <si>
     <t>李四</t>
   </si>
   <si>
@@ -94,10 +94,7 @@
     <t>餐饮</t>
   </si>
   <si>
-    <t>意向客户</t>
-  </si>
-  <si>
-    <t>food good eat</t>
+    <t>储备客户</t>
   </si>
   <si>
     <t>王五</t>
@@ -112,7 +109,7 @@
     <t>中国广州</t>
   </si>
   <si>
-    <t>众所周知，网易是一家好公司</t>
+    <t>VIP客户</t>
   </si>
 </sst>
 </file>
@@ -120,10 +117,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -163,14 +160,96 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,51 +263,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -237,54 +271,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,187 +296,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,35 +487,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,6 +501,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,15 +529,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -572,6 +540,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,6 +576,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -598,10 +595,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -610,16 +607,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -631,112 +628,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1106,8 +1103,8 @@
   <sheetPr/>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="A1:L4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3"/>
@@ -1235,12 +1232,12 @@
         <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -1249,16 +1246,16 @@
         <v>18453156456</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F4">
         <v>123456</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -1273,7 +1270,7 @@
         <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>